<commit_message>
fix validate. fix option name bug
</commit_message>
<xml_diff>
--- a/test_file/result1.xlsx
+++ b/test_file/result1.xlsx
@@ -56,7 +56,7 @@
     <t>错误原因</t>
   </si>
   <si>
-    <t>Sex必须是[男 女]中的一个</t>
+    <t>该行有数据未正确填写</t>
   </si>
 </sst>
 </file>
@@ -383,8 +383,8 @@
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="2" min="1" style="1" width="5"/>
-    <col customWidth="true" max="3" min="3" style="1" width="37"/>
+    <col customWidth="true" max="2" min="1" style="1" width="8"/>
+    <col customWidth="true" max="3" min="3" style="1" width="40"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="true">

</xml_diff>